<commit_message>
add results of experiment and multiplication
</commit_message>
<xml_diff>
--- a/Algorithm Householder/Experiments.xlsx
+++ b/Algorithm Householder/Experiments.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CC35B4-4332-45EC-9933-B2054D974A6A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C2CC87-E09D-4A63-AD85-276EF0B0E956}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Размер матрицы</t>
   </si>
   <si>
     <t>Версия "в лоб"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Время, с </t>
-  </si>
-  <si>
-    <t>Версия Z</t>
   </si>
   <si>
     <t>Версия Eigen</t>
@@ -72,6 +66,18 @@
   <si>
     <t>Больше часа</t>
   </si>
+  <si>
+    <t xml:space="preserve">Время разложения, с </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Время вычисления Q, с </t>
+  </si>
+  <si>
+    <t>Версия RowHouse</t>
+  </si>
+  <si>
+    <t>Версия с обратным накоплением</t>
+  </si>
 </sst>
 </file>
 
@@ -94,7 +100,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +110,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -120,10 +132,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -131,7 +141,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -191,12 +214,34 @@
             </a:r>
             <a:r>
               <a:rPr lang="ru-RU" baseline="0"/>
-              <a:t> размера матрицы от времени разложения</a:t>
+              <a:t> времени разложения</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t>от </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>размера матрицы</a:t>
             </a:r>
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17622164048865618"/>
+          <c:y val="3.5173160173160176E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -233,10 +278,324 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Версия "В лоб"</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Версия Eigen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$A$3,Sheet1!$A$4,Sheet1!$A$5,Sheet1!$A$6,Sheet1!$A$7,Sheet1!$A$8,Sheet1!$A$9,Sheet1!$A$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$3:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.1405699999999996E-7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1405699999999996E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1405699999999996E-7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.1967899999999996E-6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1871500000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9167900000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.4589600000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.7373499999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>1.6023099999999998E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2863-44C5-8584-446688082C71}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Версия с обратным накоплением</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$3:$H$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.5935800000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0329300000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5751000000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0187E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.63003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.22037100000000001</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.08836</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>5.2556700000000003</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>275.92200000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D9C9-4BFA-BE6B-CFDA76AA03D0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Версия RowHouse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$A$3,Sheet1!$A$4,Sheet1!$A$5,Sheet1!$A$6,Sheet1!$A$7,Sheet1!$A$8,Sheet1!$A$9,Sheet1!$A$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.7477900000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.93012E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0096399999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.07062E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1945599999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.244342</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>1.1552199999999999</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>6.7933300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2863-44C5-8584-446688082C71}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Версия "в лоб"</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -302,28 +661,28 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2.26185E-5</c:v>
+                  <c:v>1.1823300000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5188799999999998E-5</c:v>
+                  <c:v>3.2385599999999997E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0192799999999996E-5</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>1.3198400000000001E-2</c:v>
+                  <c:v>1.11036E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.9615639999999991E-3</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>0.21163299999999999</c:v>
+                  <c:v>0.118298</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>18.706900000000001</c:v>
+                  <c:v>8.6886600000000005</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>158</c:v>
+                  <c:v>103.348</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>1551.99</c:v>
+                  <c:v>1390.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -332,212 +691,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2863-44C5-8584-446688082C71}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Версия Z</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>(Sheet1!$A$3,Sheet1!$A$4,Sheet1!$A$5,Sheet1!$A$6,Sheet1!$A$7,Sheet1!$A$8,Sheet1!$A$9,Sheet1!$A$10)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$3:$D$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>3.0843300000000003E-5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0891499999999999E-5</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>1.55759E-4</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>1.3349E-2</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>0.114909</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>11.7681</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>97.456000000000003</c:v>
-                </c:pt>
-                <c:pt idx="7" formatCode="General">
-                  <c:v>768.77800000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-2863-44C5-8584-446688082C71}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Версия Eigen</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>(Sheet1!$A$3,Sheet1!$A$4,Sheet1!$A$5,Sheet1!$A$6,Sheet1!$A$7,Sheet1!$A$8,Sheet1!$A$9,Sheet1!$A$10)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>300</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>500</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$F$3:$F$10</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>4.1124900000000002E-6</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.0281200000000001E-5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5421499999999999E-6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.05619E-6</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.7759E-5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.6885100000000002E-4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.1194500000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.5773100000000002E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-2863-44C5-8584-446688082C71}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -610,8 +763,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.49901170529039318"/>
-              <c:y val="0.82617441258020619"/>
+              <c:x val="0.46628911242115678"/>
+              <c:y val="0.86946454136414775"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -806,7 +959,885 @@
       <c:spPr>
         <a:noFill/>
         <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="73000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
           <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>График зависимости</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> времени вычисления матрицы </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Q </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t>от </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>размера матрицы</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> A</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17622164048865618"/>
+          <c:y val="3.5173160173160176E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Версия Eigen</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$A$3,Sheet1!$A$4,Sheet1!$A$5,Sheet1!$A$6,Sheet1!$A$7,Sheet1!$A$8,Sheet1!$A$9,Sheet1!$A$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$3:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.6265100000000004E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6827399999999998E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.23374E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8146199999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5980799999999996E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.35716E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.65449E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.954017</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>0.220556</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5B3C-4CFB-8A24-BA2D5544795A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Версия с обратным накоплением</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$3:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>3.86571E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.35406E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6446599999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7483100000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.3635400000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>9.1995099999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.468615</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>4.1326599999999996</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>266.53500000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5B3C-4CFB-8A24-BA2D5544795A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Версия RowHouse</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$A$3,Sheet1!$A$4,Sheet1!$A$5,Sheet1!$A$6,Sheet1!$A$7,Sheet1!$A$8,Sheet1!$A$9,Sheet1!$A$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.5462000000000004E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1823300000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2666700000000003E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.8489400000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.102795</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>9.5338700000000003</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>92.855999999999995</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>746.59199999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5B3C-4CFB-8A24-BA2D5544795A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Версия "в лоб"</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Sheet1!$A$3,Sheet1!$A$4,Sheet1!$A$5,Sheet1!$A$6,Sheet1!$A$7,Sheet1!$A$8,Sheet1!$A$9,Sheet1!$A$10)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.5984000000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6963899999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8321300000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.1717600000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>9.3141399999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>11.2646</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>94.138000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>981.36199999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5B3C-4CFB-8A24-BA2D5544795A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="540320912"/>
+        <c:axId val="540318992"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="540320912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Размер</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> матрицы</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.46628911242115678"/>
+              <c:y val="0.86946454136414775"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="540318992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="540318992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ru-RU"/>
+                  <a:t>Время,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="ru-RU" baseline="0"/>
+                  <a:t> с</a:t>
+                </a:r>
+                <a:endParaRPr lang="ru-RU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ru-RU"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="540320912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="73000"/>
+            </a:schemeClr>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -926,6 +1957,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1429,188 +2500,514 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="795154" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8CFCC38-559C-478D-A99B-EC3029D281EA}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2369820" y="190500"/>
-              <a:ext cx="795154" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:d>
-                      <m:dPr>
-                        <m:begChr m:val="‖"/>
-                        <m:endChr m:val="‖"/>
-                        <m:ctrlPr>
-                          <a:rPr lang="ru-RU" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:dPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝐴</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t> −</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑄</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>∗</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑅</m:t>
-                        </m:r>
-                      </m:e>
-                    </m:d>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="ru-RU" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8CFCC38-559C-478D-A99B-EC3029D281EA}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="2369820" y="190500"/>
-              <a:ext cx="795154" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="ru-RU" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>‖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝐴 −𝑄∗𝑅</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="ru-RU" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>‖</a:t>
-              </a:r>
-              <a:endParaRPr lang="ru-RU" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1925,16 +3322,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>670560</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>975360</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1954,6 +3351,514 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="795154" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A33EE55E-9024-4C64-B836-EDB0E7D8B290}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2796540" y="190500"/>
+              <a:ext cx="795154" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="‖"/>
+                        <m:endChr m:val="‖"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="ru-RU" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐴</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t> −</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑄</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>∗</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑅</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="6" name="TextBox 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A33EE55E-9024-4C64-B836-EDB0E7D8B290}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2796540" y="190500"/>
+              <a:ext cx="795154" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>‖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐴 −𝑄∗𝑅‖</a:t>
+              </a:r>
+              <a:endParaRPr lang="ru-RU" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="795154" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7376EE41-D057-432B-977B-590C9E9CCBBF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6263640" y="182880"/>
+              <a:ext cx="795154" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:d>
+                      <m:dPr>
+                        <m:begChr m:val="‖"/>
+                        <m:endChr m:val="‖"/>
+                        <m:ctrlPr>
+                          <a:rPr kumimoji="0" lang="ru-RU" sz="1100" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0" smtClean="0">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:uLnTx/>
+                            <a:uFillTx/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:dPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0" smtClean="0">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:uLnTx/>
+                            <a:uFillTx/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝐴</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0" smtClean="0">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:uLnTx/>
+                            <a:uFillTx/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t> −</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0" smtClean="0">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:uLnTx/>
+                            <a:uFillTx/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑄</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0" smtClean="0">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:uLnTx/>
+                            <a:uFillTx/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>∗</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0" smtClean="0">
+                            <a:ln>
+                              <a:noFill/>
+                            </a:ln>
+                            <a:solidFill>
+                              <a:sysClr val="windowText" lastClr="000000"/>
+                            </a:solidFill>
+                            <a:effectLst/>
+                            <a:uLnTx/>
+                            <a:uFillTx/>
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="+mn-ea"/>
+                            <a:cs typeface="+mn-cs"/>
+                          </a:rPr>
+                          <m:t>𝑅</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:d>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr kumimoji="0" lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:uLnTx/>
+                <a:uFillTx/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7376EE41-D057-432B-977B-590C9E9CCBBF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6263640" y="182880"/>
+              <a:ext cx="795154" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr kumimoji="0" lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:uLnTx/>
+                  <a:uFillTx/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>‖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr kumimoji="0" lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:uLnTx/>
+                  <a:uFillTx/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝐴 −𝑄∗𝑅‖</a:t>
+              </a:r>
+              <a:endParaRPr kumimoji="0" lang="ru-RU" sz="1100" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:uLnTx/>
+                <a:uFillTx/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>784860</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Диаграмма 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88777047-04CB-4D24-9D1A-78AF895B3066}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2225,272 +4130,484 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" customWidth="1"/>
+    <col min="6" max="10" width="12.21875" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="8"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="2" t="s">
+      <c r="B3" s="6">
+        <v>1.1823300000000001E-5</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3.5984000000000001E-6</v>
+      </c>
+      <c r="D3" s="6">
+        <v>9.9470000000000004E-14</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1.7477900000000001E-5</v>
+      </c>
+      <c r="F3" s="6">
+        <v>5.5462000000000004E-6</v>
+      </c>
+      <c r="G3" s="6">
+        <v>8.5265099999999998E-14</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1.5935800000000001E-5</v>
+      </c>
+      <c r="I3" s="6">
+        <v>3.86571E-4</v>
+      </c>
+      <c r="J3" s="6">
+        <v>4.2632600000000003E-14</v>
+      </c>
+      <c r="K3" s="6">
+        <v>5.1405699999999996E-7</v>
+      </c>
+      <c r="L3" s="6">
+        <v>4.6265100000000004E-6</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3.2385599999999997E-5</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1.6963899999999999E-5</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2.10964E-13</v>
+      </c>
+      <c r="E4" s="6">
+        <v>2.93012E-5</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1.1823300000000001E-5</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1.4921399999999999E-13</v>
+      </c>
+      <c r="H4" s="6">
+        <v>3.0329300000000001E-5</v>
+      </c>
+      <c r="I4" s="6">
+        <v>4.35406E-4</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1.6342500000000001E-13</v>
+      </c>
+      <c r="K4" s="6">
+        <v>5.1405699999999996E-7</v>
+      </c>
+      <c r="L4" s="6">
+        <v>6.6827399999999998E-6</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>2</v>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1.11036E-4</v>
+      </c>
+      <c r="C5" s="6">
+        <v>4.8321300000000001E-5</v>
+      </c>
+      <c r="D5" s="6">
+        <v>5.5156199999999997E-13</v>
+      </c>
+      <c r="E5" s="6">
+        <v>4.0096399999999998E-5</v>
+      </c>
+      <c r="F5" s="6">
+        <v>4.2666700000000003E-5</v>
+      </c>
+      <c r="G5" s="6">
+        <v>5.6665799999999999E-13</v>
+      </c>
+      <c r="H5" s="6">
+        <v>4.5751000000000003E-5</v>
+      </c>
+      <c r="I5" s="6">
+        <v>3.6446599999999998E-4</v>
+      </c>
+      <c r="J5" s="6">
+        <v>2.5994599999999998E-13</v>
+      </c>
+      <c r="K5" s="6">
+        <v>5.1405699999999996E-7</v>
+      </c>
+      <c r="L5" s="6">
+        <v>1.23374E-5</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2.26185E-5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>9.9470000000000004E-14</v>
-      </c>
-      <c r="D3" s="1">
-        <v>3.0843300000000003E-5</v>
-      </c>
-      <c r="E3" s="1">
-        <v>8.5265099999999998E-14</v>
-      </c>
-      <c r="F3" s="1">
-        <v>4.1124900000000002E-6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>50</v>
+      </c>
+      <c r="B6" s="6">
+        <v>9.9615639999999991E-3</v>
+      </c>
+      <c r="C6" s="6">
+        <v>6.1717600000000001E-3</v>
+      </c>
+      <c r="D6" s="6">
+        <v>5.9907619999999998E-12</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2.07062E-3</v>
+      </c>
+      <c r="F6" s="6">
+        <v>5.8489400000000004E-3</v>
+      </c>
+      <c r="G6" s="6">
+        <v>6.0513799999999996E-12</v>
+      </c>
+      <c r="H6" s="6">
+        <v>2.0187E-3</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1.7483100000000001E-3</v>
+      </c>
+      <c r="J6" s="6">
+        <v>5.6153499999999999E-12</v>
+      </c>
+      <c r="K6" s="6">
+        <v>7.1967899999999996E-6</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1.8146199999999999E-4</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2.5188799999999998E-5</v>
-      </c>
-      <c r="C4" s="1">
-        <v>2.10964E-13</v>
-      </c>
-      <c r="D4" s="1">
-        <v>5.0891499999999999E-5</v>
-      </c>
-      <c r="E4" s="1">
-        <v>1.4921399999999999E-13</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1.0281200000000001E-5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>100</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.118298</v>
+      </c>
+      <c r="C7" s="9">
+        <v>9.3141399999999999E-2</v>
+      </c>
+      <c r="D7" s="6">
+        <v>9.8398699999999993E-12</v>
+      </c>
+      <c r="E7" s="6">
+        <v>2.1945599999999999E-2</v>
+      </c>
+      <c r="F7" s="6">
+        <v>0.102795</v>
+      </c>
+      <c r="G7" s="6">
+        <v>2.4011900000000001E-11</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1.63003E-2</v>
+      </c>
+      <c r="I7" s="6">
+        <v>9.3635400000000001E-3</v>
+      </c>
+      <c r="J7" s="6">
+        <v>3.4472899999999999E-11</v>
+      </c>
+      <c r="K7" s="6">
+        <v>3.1871500000000001E-5</v>
+      </c>
+      <c r="L7" s="6">
+        <v>5.5980799999999996E-4</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>300</v>
+      </c>
+      <c r="B8" s="2">
+        <v>8.6886600000000005</v>
+      </c>
+      <c r="C8" s="9">
+        <v>11.2646</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1.1290000000000001E-10</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.244342</v>
+      </c>
+      <c r="F8" s="2">
+        <v>9.5338700000000003</v>
+      </c>
+      <c r="G8" s="6">
+        <v>9.1564E-11</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.22037100000000001</v>
+      </c>
+      <c r="I8" s="2">
+        <v>9.1995099999999996E-2</v>
+      </c>
+      <c r="J8" s="6">
+        <v>8.5905E-11</v>
+      </c>
+      <c r="K8" s="6">
+        <v>5.9167900000000001E-4</v>
+      </c>
+      <c r="L8" s="6">
+        <v>1.35716E-2</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>500</v>
+      </c>
+      <c r="B9" s="2">
+        <v>103.348</v>
+      </c>
+      <c r="C9" s="9">
+        <v>94.138000000000005</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2.7636899999999999E-10</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.1552199999999999</v>
+      </c>
+      <c r="F9" s="2">
+        <v>92.855999999999995</v>
+      </c>
+      <c r="G9" s="6">
+        <v>3.0140600000000001E-10</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.08836</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.468615</v>
+      </c>
+      <c r="J9" s="6">
+        <v>4.4542200000000002E-10</v>
+      </c>
+      <c r="K9" s="6">
+        <v>7.4589600000000002E-4</v>
+      </c>
+      <c r="L9" s="6">
+        <v>2.65449E-2</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>800</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1390.83</v>
+      </c>
+      <c r="C10" s="9">
+        <v>981.36199999999997</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5.0763299999999996E-10</v>
+      </c>
+      <c r="E10" s="2">
+        <v>6.7933300000000001</v>
+      </c>
+      <c r="F10" s="2">
+        <v>746.59199999999998</v>
+      </c>
+      <c r="G10" s="6">
+        <v>5.6068999999999995E-10</v>
+      </c>
+      <c r="H10" s="2">
+        <v>5.2556700000000003</v>
+      </c>
+      <c r="I10" s="2">
+        <v>4.1326599999999996</v>
+      </c>
+      <c r="J10" s="6">
+        <v>5.2246000000000003E-9</v>
+      </c>
+      <c r="K10" s="6">
+        <v>2.7373499999999999E-3</v>
+      </c>
+      <c r="L10" s="6">
+        <v>0.954017</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="2">
+        <v>275.92200000000003</v>
+      </c>
+      <c r="I11" s="2">
+        <v>266.53500000000003</v>
+      </c>
+      <c r="J11" s="6">
+        <v>2.14322E-9</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1.6023099999999998E-2</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.220556</v>
+      </c>
+      <c r="M11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
-        <v>8.0192799999999996E-5</v>
-      </c>
-      <c r="C5" s="1">
-        <v>5.5156199999999997E-13</v>
-      </c>
-      <c r="D5">
-        <v>1.55759E-4</v>
-      </c>
-      <c r="E5" s="1">
-        <v>5.6665799999999999E-13</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1.5421499999999999E-6</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>50</v>
-      </c>
-      <c r="B6">
-        <v>1.3198400000000001E-2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>5.9907619999999998E-12</v>
-      </c>
-      <c r="D6">
-        <v>1.3349E-2</v>
-      </c>
-      <c r="E6" s="1">
-        <v>6.0513799999999996E-12</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2.05619E-6</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>1500</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3">
-        <v>100</v>
-      </c>
-      <c r="B7">
-        <v>0.21163299999999999</v>
-      </c>
-      <c r="C7" s="1">
-        <v>9.8398699999999993E-12</v>
-      </c>
-      <c r="D7">
-        <v>0.114909</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2.4011900000000001E-11</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2.7759E-5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>300</v>
-      </c>
-      <c r="B8">
-        <v>18.706900000000001</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1.1290000000000001E-10</v>
-      </c>
-      <c r="D8">
-        <v>11.7681</v>
-      </c>
-      <c r="E8" s="1">
-        <v>9.1564E-11</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2.6885100000000002E-4</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>500</v>
-      </c>
-      <c r="B9">
-        <v>158</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2.7636899999999999E-10</v>
-      </c>
-      <c r="D9">
-        <v>97.456000000000003</v>
-      </c>
-      <c r="E9" s="1">
-        <v>3.0140600000000001E-10</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2.1194500000000002E-3</v>
-      </c>
-      <c r="G9" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>2000</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>800</v>
-      </c>
-      <c r="B10">
-        <v>1551.99</v>
-      </c>
-      <c r="C10" s="1">
-        <v>5.0763299999999996E-10</v>
-      </c>
-      <c r="D10">
-        <v>768.77800000000002</v>
-      </c>
-      <c r="E10" s="1">
-        <v>5.6068999999999995E-10</v>
-      </c>
-      <c r="F10" s="1">
-        <v>3.5773100000000002E-3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
-        <v>1000</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>1500</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
-      <c r="G12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>2000</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
-      <c r="G13" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
+  <mergeCells count="5">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B11:G13"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>